<commit_message>
Revert "create bootstrap replicates"
This reverts commit 87d736d8b3308dacf3fa841adf1193afa0e12875.
</commit_message>
<xml_diff>
--- a/Data/male_AngII_data.xlsx
+++ b/Data/male_AngII_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s347ahme/Documents/GitHub/BP-Regulation/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s347ahme/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9A2844-D74C-5349-B87B-239B1E10C0AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B5428F7-EA99-7F43-B491-AC9E1B5EA9BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19180" windowHeight="10060" xr2:uid="{43CE0AE6-412E-2D40-A40B-86CF135EB9AB}"/>
+    <workbookView xWindow="19220" yWindow="460" windowWidth="19180" windowHeight="10060" xr2:uid="{43CE0AE6-412E-2D40-A40B-86CF135EB9AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,17 +30,9 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>Rat/Day</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -52,14 +44,6 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -82,12 +66,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,296 +385,293 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72AA4AB7-8CB2-F343-9A30-D1685D659729}">
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22:F23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" s="1">
+        <v>139.20031122217171</v>
+      </c>
+      <c r="B1" s="1">
+        <v>140.34202857142861</v>
+      </c>
+      <c r="C1" s="1">
+        <v>149.40688194444442</v>
+      </c>
+      <c r="D1" s="1">
+        <v>157.07371646825396</v>
+      </c>
+      <c r="E1" s="1">
+        <v>164.73983333333334</v>
+      </c>
+      <c r="F1" s="1">
+        <v>160.03967899786778</v>
+      </c>
+      <c r="G1" s="1">
+        <v>175.76867361111107</v>
+      </c>
+      <c r="H1" s="1">
+        <v>175.3147083333333</v>
+      </c>
+      <c r="I1" s="1">
+        <v>175.52218427230048</v>
+      </c>
+      <c r="J1" s="1">
+        <v>173.70881944444437</v>
+      </c>
+      <c r="K1" s="1">
+        <v>169.13554003267976</v>
+      </c>
+      <c r="L1" s="1">
+        <v>161.66354370915036</v>
+      </c>
+      <c r="M1" s="1">
+        <v>170.88670519713258</v>
+      </c>
+      <c r="N1" s="1">
+        <v>175.76210542929294</v>
+      </c>
+      <c r="O1" s="1">
+        <v>178.32979245283011</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>143.9605745305164</v>
+      </c>
       <c r="B2" s="1">
-        <v>139.20031122217171</v>
+        <v>140.3512875586855</v>
       </c>
       <c r="C2" s="1">
-        <v>140.34202857142861</v>
+        <v>153.75590972222227</v>
       </c>
       <c r="D2" s="1">
-        <v>149.40688194444442</v>
+        <v>166.12080829420972</v>
       </c>
       <c r="E2" s="1">
-        <v>157.07371646825396</v>
+        <v>172.24829285714281</v>
       </c>
       <c r="F2" s="1">
-        <v>164.73983333333334</v>
+        <v>180.09930465401109</v>
       </c>
       <c r="G2" s="1">
-        <v>160.03967899786778</v>
+        <v>168.99818749999997</v>
       </c>
       <c r="H2" s="1">
-        <v>175.76867361111107</v>
+        <v>157.32905164319254</v>
       </c>
       <c r="I2" s="1">
-        <v>175.3147083333333</v>
+        <v>180.58776486697968</v>
       </c>
       <c r="J2" s="1">
-        <v>175.52218427230048</v>
+        <v>174.14202014866976</v>
       </c>
       <c r="K2" s="1">
-        <v>173.70881944444437</v>
+        <v>183.70036551251957</v>
       </c>
       <c r="L2" s="1">
-        <v>169.13554003267976</v>
+        <v>179.83996840766827</v>
       </c>
       <c r="M2" s="1">
-        <v>161.66354370915036</v>
+        <v>188.34129438405796</v>
       </c>
       <c r="N2" s="1">
-        <v>170.88670519713258</v>
+        <v>191.4669375</v>
       </c>
       <c r="O2" s="1">
-        <v>175.76210542929294</v>
-      </c>
-      <c r="P2" s="1">
-        <v>178.32979245283011</v>
+        <v>198.29475471698109</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>139.81887499999999</v>
+      </c>
       <c r="B3" s="1">
-        <v>143.9605745305164</v>
+        <v>143.21271527777782</v>
       </c>
       <c r="C3" s="1">
-        <v>140.3512875586855</v>
+        <v>145.6477292644758</v>
       </c>
       <c r="D3" s="1">
-        <v>153.75590972222227</v>
+        <v>154.09429861111113</v>
       </c>
       <c r="E3" s="1">
-        <v>166.12080829420972</v>
+        <v>157.77694444444444</v>
       </c>
       <c r="F3" s="1">
-        <v>172.24829285714281</v>
+        <v>167.57557638888886</v>
       </c>
       <c r="G3" s="1">
-        <v>180.09930465401109</v>
+        <v>170.54908091787439</v>
       </c>
       <c r="H3" s="1">
-        <v>168.99818749999997</v>
+        <v>174.2655352112676</v>
       </c>
       <c r="I3" s="1">
-        <v>157.32905164319254</v>
+        <v>178.85754914529912</v>
       </c>
       <c r="J3" s="1">
-        <v>180.58776486697968</v>
+        <v>188.09036766431925</v>
       </c>
       <c r="K3" s="1">
-        <v>174.14202014866976</v>
+        <v>189.74308423913044</v>
       </c>
       <c r="L3" s="1">
-        <v>183.70036551251957</v>
+        <v>194.17318750000007</v>
       </c>
       <c r="M3" s="1">
-        <v>179.83996840766827</v>
+        <v>190.67703234126986</v>
       </c>
       <c r="N3" s="1">
-        <v>188.34129438405796</v>
+        <v>194.67494957729468</v>
       </c>
       <c r="O3" s="1">
-        <v>191.4669375</v>
-      </c>
-      <c r="P3" s="1">
-        <v>198.29475471698109</v>
+        <v>181.59151020408163</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>156.002222222222</v>
+      </c>
       <c r="B4" s="1">
-        <v>139.81887499999999</v>
+        <v>150.92110416666699</v>
       </c>
       <c r="C4" s="1">
-        <v>143.21271527777782</v>
+        <v>153.870427696078</v>
       </c>
       <c r="D4" s="1">
-        <v>145.6477292644758</v>
+        <v>154.65341625817001</v>
       </c>
       <c r="E4" s="1">
-        <v>154.09429861111113</v>
+        <v>153.17024448181601</v>
       </c>
       <c r="F4" s="1">
-        <v>157.77694444444444</v>
+        <v>147.40513888888893</v>
       </c>
       <c r="G4" s="1">
-        <v>167.57557638888886</v>
+        <v>150.37109027777774</v>
       </c>
       <c r="H4" s="1">
-        <v>170.54908091787439</v>
+        <v>156.35045833333336</v>
       </c>
       <c r="I4" s="1">
-        <v>174.2655352112676</v>
+        <v>165.38011805555556</v>
       </c>
       <c r="J4" s="1">
-        <v>178.85754914529912</v>
+        <v>168.74470833333334</v>
       </c>
       <c r="K4" s="1">
-        <v>188.09036766431925</v>
+        <v>168.55970996732026</v>
       </c>
       <c r="L4" s="1">
-        <v>189.74308423913044</v>
+        <v>173.43204166666669</v>
       </c>
       <c r="M4" s="1">
-        <v>194.17318750000007</v>
+        <v>179.41530595882989</v>
       </c>
       <c r="N4" s="1">
-        <v>190.67703234126986</v>
+        <v>177.97422222222221</v>
       </c>
       <c r="O4" s="1">
-        <v>194.67494957729468</v>
-      </c>
-      <c r="P4" s="1">
-        <v>181.59151020408163</v>
+        <v>182.9022745098039</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>155.99386111111113</v>
+      </c>
       <c r="B5" s="1">
-        <v>156.002222222222</v>
+        <v>164.46365277777775</v>
       </c>
       <c r="C5" s="1">
-        <v>150.92110416666699</v>
+        <v>155.74509154929575</v>
       </c>
       <c r="D5" s="1">
-        <v>153.870427696078</v>
+        <v>163.31999264705883</v>
       </c>
       <c r="E5" s="1">
-        <v>154.65341625817001</v>
+        <v>170.44788749999998</v>
       </c>
       <c r="F5" s="1">
-        <v>153.17024448181601</v>
+        <v>170.55326251956183</v>
       </c>
       <c r="G5" s="1">
-        <v>147.40513888888893</v>
+        <v>175.73152777777779</v>
       </c>
       <c r="H5" s="1">
-        <v>150.37109027777774</v>
+        <v>176.2855528169014</v>
       </c>
       <c r="I5" s="1">
-        <v>156.35045833333336</v>
+        <v>178.89197222222222</v>
       </c>
       <c r="J5" s="1">
-        <v>165.38011805555556</v>
+        <v>184.8161527777778</v>
       </c>
       <c r="K5" s="1">
-        <v>168.74470833333334</v>
+        <v>182.2265902777778</v>
       </c>
       <c r="L5" s="1">
-        <v>168.55970996732026</v>
+        <v>193.97030827294691</v>
       </c>
       <c r="M5" s="1">
-        <v>173.43204166666669</v>
+        <v>192.29093613067295</v>
       </c>
       <c r="N5" s="1">
-        <v>179.41530595882989</v>
+        <v>201.65639239850873</v>
       </c>
       <c r="O5" s="1">
-        <v>177.97422222222221</v>
-      </c>
-      <c r="P5" s="1">
-        <v>182.9022745098039</v>
+        <v>195.80447999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>143.92815463615025</v>
+      </c>
       <c r="B6" s="1">
-        <v>155.99386111111113</v>
+        <v>150.96643055555558</v>
       </c>
       <c r="C6" s="1">
-        <v>164.46365277777775</v>
+        <v>152.41623611111106</v>
       </c>
       <c r="D6" s="1">
-        <v>155.74509154929575</v>
+        <v>155.45623611111114</v>
       </c>
       <c r="E6" s="1">
-        <v>163.31999264705883</v>
+        <v>161.84281944444439</v>
       </c>
       <c r="F6" s="1">
-        <v>170.44788749999998</v>
+        <v>161.50074559859155</v>
       </c>
       <c r="G6" s="1">
-        <v>170.55326251956183</v>
+        <v>172.72622916666671</v>
       </c>
       <c r="H6" s="1">
-        <v>175.73152777777779</v>
+        <v>173.18365972222225</v>
       </c>
       <c r="I6" s="1">
-        <v>176.2855528169014</v>
+        <v>168.45324520735525</v>
       </c>
       <c r="J6" s="1">
-        <v>178.89197222222222</v>
+        <v>175.15825694444445</v>
       </c>
       <c r="K6" s="1">
-        <v>184.8161527777778</v>
+        <v>169.51418055555558</v>
       </c>
       <c r="L6" s="1">
-        <v>182.2265902777778</v>
+        <v>170.8078888888889</v>
       </c>
       <c r="M6" s="1">
-        <v>193.97030827294691</v>
+        <v>179.3271527777778</v>
       </c>
       <c r="N6" s="1">
-        <v>192.29093613067295</v>
+        <v>184.73595328282823</v>
       </c>
       <c r="O6" s="1">
-        <v>201.65639239850873</v>
-      </c>
-      <c r="P6" s="1">
-        <v>195.80447999999996</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B7" s="1">
-        <v>143.92815463615025</v>
-      </c>
-      <c r="C7" s="1">
-        <v>150.96643055555558</v>
-      </c>
-      <c r="D7" s="1">
-        <v>152.41623611111106</v>
-      </c>
-      <c r="E7" s="1">
-        <v>155.45623611111114</v>
-      </c>
-      <c r="F7" s="1">
-        <v>161.84281944444439</v>
-      </c>
-      <c r="G7" s="1">
-        <v>161.50074559859155</v>
-      </c>
-      <c r="H7" s="1">
-        <v>172.72622916666671</v>
-      </c>
-      <c r="I7" s="1">
-        <v>173.18365972222225</v>
-      </c>
-      <c r="J7" s="1">
-        <v>168.45324520735525</v>
-      </c>
-      <c r="K7" s="1">
-        <v>175.15825694444445</v>
-      </c>
-      <c r="L7" s="1">
-        <v>169.51418055555558</v>
-      </c>
-      <c r="M7" s="1">
-        <v>170.8078888888889</v>
-      </c>
-      <c r="N7" s="1">
-        <v>179.3271527777778</v>
-      </c>
-      <c r="O7" s="1">
-        <v>184.73595328282823</v>
-      </c>
-      <c r="P7" s="1">
         <v>181.71616981132075</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "Revert "create bootstrap replicates""
This reverts commit e1f04f71f72b4138ce8cc5c0c59bb757fb6379ae.
</commit_message>
<xml_diff>
--- a/Data/male_AngII_data.xlsx
+++ b/Data/male_AngII_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s347ahme/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s347ahme/Documents/GitHub/BP-Regulation/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B5428F7-EA99-7F43-B491-AC9E1B5EA9BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9A2844-D74C-5349-B87B-239B1E10C0AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19220" yWindow="460" windowWidth="19180" windowHeight="10060" xr2:uid="{43CE0AE6-412E-2D40-A40B-86CF135EB9AB}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19180" windowHeight="10060" xr2:uid="{43CE0AE6-412E-2D40-A40B-86CF135EB9AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,9 +30,17 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>Rat/Day</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -44,6 +52,14 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -66,11 +82,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -385,293 +402,296 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72AA4AB7-8CB2-F343-9A30-D1685D659729}">
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22:F23"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="1">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B2" s="1">
         <v>139.20031122217171</v>
       </c>
-      <c r="B1" s="1">
+      <c r="C2" s="1">
         <v>140.34202857142861</v>
       </c>
-      <c r="C1" s="1">
+      <c r="D2" s="1">
         <v>149.40688194444442</v>
       </c>
-      <c r="D1" s="1">
+      <c r="E2" s="1">
         <v>157.07371646825396</v>
       </c>
-      <c r="E1" s="1">
+      <c r="F2" s="1">
         <v>164.73983333333334</v>
       </c>
-      <c r="F1" s="1">
+      <c r="G2" s="1">
         <v>160.03967899786778</v>
       </c>
-      <c r="G1" s="1">
+      <c r="H2" s="1">
         <v>175.76867361111107</v>
       </c>
-      <c r="H1" s="1">
+      <c r="I2" s="1">
         <v>175.3147083333333</v>
       </c>
-      <c r="I1" s="1">
+      <c r="J2" s="1">
         <v>175.52218427230048</v>
       </c>
-      <c r="J1" s="1">
+      <c r="K2" s="1">
         <v>173.70881944444437</v>
       </c>
-      <c r="K1" s="1">
+      <c r="L2" s="1">
         <v>169.13554003267976</v>
       </c>
-      <c r="L1" s="1">
+      <c r="M2" s="1">
         <v>161.66354370915036</v>
       </c>
-      <c r="M1" s="1">
+      <c r="N2" s="1">
         <v>170.88670519713258</v>
       </c>
-      <c r="N1" s="1">
+      <c r="O2" s="1">
         <v>175.76210542929294</v>
       </c>
-      <c r="O1" s="1">
+      <c r="P2" s="1">
         <v>178.32979245283011</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B3" s="1">
         <v>143.9605745305164</v>
       </c>
-      <c r="B2" s="1">
+      <c r="C3" s="1">
         <v>140.3512875586855</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D3" s="1">
         <v>153.75590972222227</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E3" s="1">
         <v>166.12080829420972</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F3" s="1">
         <v>172.24829285714281</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G3" s="1">
         <v>180.09930465401109</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H3" s="1">
         <v>168.99818749999997</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I3" s="1">
         <v>157.32905164319254</v>
       </c>
-      <c r="I2" s="1">
+      <c r="J3" s="1">
         <v>180.58776486697968</v>
       </c>
-      <c r="J2" s="1">
+      <c r="K3" s="1">
         <v>174.14202014866976</v>
       </c>
-      <c r="K2" s="1">
+      <c r="L3" s="1">
         <v>183.70036551251957</v>
       </c>
-      <c r="L2" s="1">
+      <c r="M3" s="1">
         <v>179.83996840766827</v>
       </c>
-      <c r="M2" s="1">
+      <c r="N3" s="1">
         <v>188.34129438405796</v>
       </c>
-      <c r="N2" s="1">
+      <c r="O3" s="1">
         <v>191.4669375</v>
       </c>
-      <c r="O2" s="1">
+      <c r="P3" s="1">
         <v>198.29475471698109</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B4" s="1">
         <v>139.81887499999999</v>
       </c>
-      <c r="B3" s="1">
+      <c r="C4" s="1">
         <v>143.21271527777782</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D4" s="1">
         <v>145.6477292644758</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E4" s="1">
         <v>154.09429861111113</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F4" s="1">
         <v>157.77694444444444</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G4" s="1">
         <v>167.57557638888886</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H4" s="1">
         <v>170.54908091787439</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I4" s="1">
         <v>174.2655352112676</v>
       </c>
-      <c r="I3" s="1">
+      <c r="J4" s="1">
         <v>178.85754914529912</v>
       </c>
-      <c r="J3" s="1">
+      <c r="K4" s="1">
         <v>188.09036766431925</v>
       </c>
-      <c r="K3" s="1">
+      <c r="L4" s="1">
         <v>189.74308423913044</v>
       </c>
-      <c r="L3" s="1">
+      <c r="M4" s="1">
         <v>194.17318750000007</v>
       </c>
-      <c r="M3" s="1">
+      <c r="N4" s="1">
         <v>190.67703234126986</v>
       </c>
-      <c r="N3" s="1">
+      <c r="O4" s="1">
         <v>194.67494957729468</v>
       </c>
-      <c r="O3" s="1">
+      <c r="P4" s="1">
         <v>181.59151020408163</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B5" s="1">
         <v>156.002222222222</v>
       </c>
-      <c r="B4" s="1">
+      <c r="C5" s="1">
         <v>150.92110416666699</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D5" s="1">
         <v>153.870427696078</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E5" s="1">
         <v>154.65341625817001</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F5" s="1">
         <v>153.17024448181601</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G5" s="1">
         <v>147.40513888888893</v>
       </c>
-      <c r="G4" s="1">
+      <c r="H5" s="1">
         <v>150.37109027777774</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I5" s="1">
         <v>156.35045833333336</v>
       </c>
-      <c r="I4" s="1">
+      <c r="J5" s="1">
         <v>165.38011805555556</v>
       </c>
-      <c r="J4" s="1">
+      <c r="K5" s="1">
         <v>168.74470833333334</v>
       </c>
-      <c r="K4" s="1">
+      <c r="L5" s="1">
         <v>168.55970996732026</v>
       </c>
-      <c r="L4" s="1">
+      <c r="M5" s="1">
         <v>173.43204166666669</v>
       </c>
-      <c r="M4" s="1">
+      <c r="N5" s="1">
         <v>179.41530595882989</v>
       </c>
-      <c r="N4" s="1">
+      <c r="O5" s="1">
         <v>177.97422222222221</v>
       </c>
-      <c r="O4" s="1">
+      <c r="P5" s="1">
         <v>182.9022745098039</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B6" s="1">
         <v>155.99386111111113</v>
       </c>
-      <c r="B5" s="1">
+      <c r="C6" s="1">
         <v>164.46365277777775</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D6" s="1">
         <v>155.74509154929575</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E6" s="1">
         <v>163.31999264705883</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F6" s="1">
         <v>170.44788749999998</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G6" s="1">
         <v>170.55326251956183</v>
       </c>
-      <c r="G5" s="1">
+      <c r="H6" s="1">
         <v>175.73152777777779</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I6" s="1">
         <v>176.2855528169014</v>
       </c>
-      <c r="I5" s="1">
+      <c r="J6" s="1">
         <v>178.89197222222222</v>
       </c>
-      <c r="J5" s="1">
+      <c r="K6" s="1">
         <v>184.8161527777778</v>
       </c>
-      <c r="K5" s="1">
+      <c r="L6" s="1">
         <v>182.2265902777778</v>
       </c>
-      <c r="L5" s="1">
+      <c r="M6" s="1">
         <v>193.97030827294691</v>
       </c>
-      <c r="M5" s="1">
+      <c r="N6" s="1">
         <v>192.29093613067295</v>
       </c>
-      <c r="N5" s="1">
+      <c r="O6" s="1">
         <v>201.65639239850873</v>
       </c>
-      <c r="O5" s="1">
+      <c r="P6" s="1">
         <v>195.80447999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B7" s="1">
         <v>143.92815463615025</v>
       </c>
-      <c r="B6" s="1">
+      <c r="C7" s="1">
         <v>150.96643055555558</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D7" s="1">
         <v>152.41623611111106</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E7" s="1">
         <v>155.45623611111114</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F7" s="1">
         <v>161.84281944444439</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G7" s="1">
         <v>161.50074559859155</v>
       </c>
-      <c r="G6" s="1">
+      <c r="H7" s="1">
         <v>172.72622916666671</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I7" s="1">
         <v>173.18365972222225</v>
       </c>
-      <c r="I6" s="1">
+      <c r="J7" s="1">
         <v>168.45324520735525</v>
       </c>
-      <c r="J6" s="1">
+      <c r="K7" s="1">
         <v>175.15825694444445</v>
       </c>
-      <c r="K6" s="1">
+      <c r="L7" s="1">
         <v>169.51418055555558</v>
       </c>
-      <c r="L6" s="1">
+      <c r="M7" s="1">
         <v>170.8078888888889</v>
       </c>
-      <c r="M6" s="1">
+      <c r="N7" s="1">
         <v>179.3271527777778</v>
       </c>
-      <c r="N6" s="1">
+      <c r="O7" s="1">
         <v>184.73595328282823</v>
       </c>
-      <c r="O6" s="1">
+      <c r="P7" s="1">
         <v>181.71616981132075</v>
       </c>
     </row>

</xml_diff>